<commit_message>
Criação dos shapefiles com as contagens de espécies de invertebrados
</commit_message>
<xml_diff>
--- a/invertebrados/ocorrencias/Validado_Gastropoda_consolidado_05abr23.xlsx
+++ b/invertebrados/ocorrencias/Validado_Gastropoda_consolidado_05abr23.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Taise\bluePrintAraguaia\Dados\Invertebrados\gastropoda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Taise\mapasAraguaia\invertebrados\ocorrencias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A355FB9D-611D-4C6D-AA2B-D24B490499AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F64329-892C-4BB9-B265-9BA90077C1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1542,7 +1542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1550,7 +1550,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1867,8 +1866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AL9" sqref="AL9"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Z45" sqref="Z45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4555,7 +4554,6 @@
       <c r="AH29" t="s">
         <v>79</v>
       </c>
-      <c r="AI29" s="7"/>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -4648,7 +4646,6 @@
       <c r="AH30" t="s">
         <v>79</v>
       </c>
-      <c r="AI30" s="7"/>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -4708,7 +4705,6 @@
       <c r="AH31" t="s">
         <v>426</v>
       </c>
-      <c r="AI31" s="7"/>
       <c r="AK31" t="s">
         <v>79</v>
       </c>
@@ -5844,8 +5840,8 @@
       <c r="Y45" t="s">
         <v>25</v>
       </c>
-      <c r="Z45" t="s">
-        <v>397</v>
+      <c r="Z45" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="AC45" t="s">
         <v>392</v>

</xml_diff>